<commit_message>
alteração no arquivo do google e tratado coisa simples
</commit_message>
<xml_diff>
--- a/src/files/notas_filmes.xlsx
+++ b/src/files/notas_filmes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J151"/>
+  <dimension ref="A1:J197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4823,6 +4823,1258 @@
       <c r="I151" t="inlineStr"/>
       <c r="J151" t="inlineStr"/>
     </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Sexta feira 13 parte 5</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>7,5</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr"/>
+      <c r="F152" t="inlineStr"/>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" t="inlineStr"/>
+      <c r="I152" t="inlineStr"/>
+      <c r="J152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Sexta feira 13 parte 6</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr"/>
+      <c r="F153" t="inlineStr"/>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" t="inlineStr"/>
+      <c r="I153" t="inlineStr"/>
+      <c r="J153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Sexta feira 13 parte 7</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>7,5</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr"/>
+      <c r="F154" t="inlineStr"/>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" t="inlineStr"/>
+      <c r="I154" t="inlineStr"/>
+      <c r="J154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Sexta feira 13 parte 8</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr"/>
+      <c r="F155" t="inlineStr"/>
+      <c r="G155" t="inlineStr"/>
+      <c r="H155" t="inlineStr"/>
+      <c r="I155" t="inlineStr"/>
+      <c r="J155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Sexta feira 13 parte 9</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr"/>
+      <c r="F156" t="inlineStr"/>
+      <c r="G156" t="inlineStr"/>
+      <c r="H156" t="inlineStr"/>
+      <c r="I156" t="inlineStr"/>
+      <c r="J156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Sexta feira 13 parte 10</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr"/>
+      <c r="F157" t="inlineStr"/>
+      <c r="G157" t="inlineStr"/>
+      <c r="H157" t="inlineStr"/>
+      <c r="I157" t="inlineStr"/>
+      <c r="J157" t="inlineStr"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Sexta feira 13 parte 11</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr"/>
+      <c r="F158" t="inlineStr"/>
+      <c r="G158" t="inlineStr"/>
+      <c r="H158" t="inlineStr"/>
+      <c r="I158" t="inlineStr"/>
+      <c r="J158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Sexta feira 13 remake</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr"/>
+      <c r="F159" t="inlineStr"/>
+      <c r="G159" t="inlineStr"/>
+      <c r="H159" t="inlineStr"/>
+      <c r="I159" t="inlineStr"/>
+      <c r="J159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Halloween</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr"/>
+      <c r="F160" t="inlineStr"/>
+      <c r="G160" t="inlineStr"/>
+      <c r="H160" t="inlineStr"/>
+      <c r="I160" t="inlineStr"/>
+      <c r="J160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Halloween 2</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr"/>
+      <c r="F161" t="inlineStr"/>
+      <c r="G161" t="inlineStr"/>
+      <c r="H161" t="inlineStr"/>
+      <c r="I161" t="inlineStr"/>
+      <c r="J161" t="inlineStr"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Halloween 3</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>6,5</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr"/>
+      <c r="F162" t="inlineStr"/>
+      <c r="G162" t="inlineStr"/>
+      <c r="H162" t="inlineStr"/>
+      <c r="I162" t="inlineStr"/>
+      <c r="J162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Halloween 4</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr"/>
+      <c r="F163" t="inlineStr"/>
+      <c r="G163" t="inlineStr"/>
+      <c r="H163" t="inlineStr"/>
+      <c r="I163" t="inlineStr"/>
+      <c r="J163" t="inlineStr"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Halloween 5</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>6,5</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr"/>
+      <c r="F164" t="inlineStr"/>
+      <c r="G164" t="inlineStr"/>
+      <c r="H164" t="inlineStr"/>
+      <c r="I164" t="inlineStr"/>
+      <c r="J164" t="inlineStr"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Halloween 6</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>6,5</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr"/>
+      <c r="F165" t="inlineStr"/>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" t="inlineStr"/>
+      <c r="I165" t="inlineStr"/>
+      <c r="J165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Halloween remake 1</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>7,5</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr"/>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" t="inlineStr"/>
+      <c r="I166" t="inlineStr"/>
+      <c r="J166" t="inlineStr"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Donnie darko</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr"/>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr"/>
+      <c r="H167" t="inlineStr"/>
+      <c r="I167" t="inlineStr"/>
+      <c r="J167" t="inlineStr"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Halloween remake 2</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>5,5</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr"/>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr"/>
+      <c r="H168" t="inlineStr"/>
+      <c r="I168" t="inlineStr"/>
+      <c r="J168" t="inlineStr"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Halloween remake (2018)</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>9,5</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr"/>
+      <c r="F169" t="inlineStr"/>
+      <c r="G169" t="inlineStr"/>
+      <c r="H169" t="inlineStr"/>
+      <c r="I169" t="inlineStr"/>
+      <c r="J169" t="inlineStr"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>predador</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr"/>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>6,5</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J170" t="inlineStr"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>predador 2</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr"/>
+      <c r="F171" t="inlineStr"/>
+      <c r="G171" t="inlineStr"/>
+      <c r="H171" t="inlineStr"/>
+      <c r="I171" t="inlineStr"/>
+      <c r="J171" t="inlineStr"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>alien</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>7,5</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr"/>
+      <c r="F172" t="inlineStr"/>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr"/>
+      <c r="I172" t="inlineStr"/>
+      <c r="J172" t="inlineStr"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>alien 2</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>7,5</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>7,5</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr"/>
+      <c r="F173" t="inlineStr"/>
+      <c r="G173" t="inlineStr"/>
+      <c r="H173" t="inlineStr"/>
+      <c r="I173" t="inlineStr"/>
+      <c r="J173" t="inlineStr"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>alien 3</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr"/>
+      <c r="F174" t="inlineStr"/>
+      <c r="G174" t="inlineStr"/>
+      <c r="H174" t="inlineStr"/>
+      <c r="I174" t="inlineStr"/>
+      <c r="J174" t="inlineStr"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>alien 4</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>3,5</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr"/>
+      <c r="F175" t="inlineStr"/>
+      <c r="G175" t="inlineStr"/>
+      <c r="H175" t="inlineStr"/>
+      <c r="I175" t="inlineStr"/>
+      <c r="J175" t="inlineStr"/>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>alien vs predador</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr"/>
+      <c r="F176" t="inlineStr"/>
+      <c r="G176" t="inlineStr"/>
+      <c r="H176" t="inlineStr"/>
+      <c r="I176" t="inlineStr"/>
+      <c r="J176" t="inlineStr"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>alien vs predador 2</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr"/>
+      <c r="F177" t="inlineStr"/>
+      <c r="G177" t="inlineStr"/>
+      <c r="H177" t="inlineStr"/>
+      <c r="I177" t="inlineStr"/>
+      <c r="J177" t="inlineStr"/>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>a morte de stalin</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr"/>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr"/>
+      <c r="H178" t="inlineStr"/>
+      <c r="I178" t="inlineStr"/>
+      <c r="J178" t="inlineStr"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>nosferatu</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr"/>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr"/>
+      <c r="H179" t="inlineStr"/>
+      <c r="I179" t="inlineStr"/>
+      <c r="J179" t="inlineStr"/>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>the trip</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr"/>
+      <c r="F180" t="inlineStr"/>
+      <c r="G180" t="inlineStr"/>
+      <c r="H180" t="inlineStr"/>
+      <c r="I180" t="inlineStr"/>
+      <c r="J180" t="inlineStr"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>encontro de casais</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr"/>
+      <c r="F181" t="inlineStr"/>
+      <c r="G181" t="inlineStr"/>
+      <c r="H181" t="inlineStr"/>
+      <c r="I181" t="inlineStr"/>
+      <c r="J181" t="inlineStr"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>o baba(ca)</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr"/>
+      <c r="F182" t="inlineStr"/>
+      <c r="G182" t="inlineStr"/>
+      <c r="H182" t="inlineStr"/>
+      <c r="I182" t="inlineStr"/>
+      <c r="J182" t="inlineStr"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>os caça-noivas</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr"/>
+      <c r="F183" t="inlineStr"/>
+      <c r="G183" t="inlineStr"/>
+      <c r="H183" t="inlineStr"/>
+      <c r="I183" t="inlineStr"/>
+      <c r="J183" t="inlineStr"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>a ressaca</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>7,5</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr"/>
+      <c r="F184" t="inlineStr"/>
+      <c r="G184" t="inlineStr"/>
+      <c r="H184" t="inlineStr"/>
+      <c r="I184" t="inlineStr"/>
+      <c r="J184" t="inlineStr"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>a ressaca 2</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>pútrido</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr"/>
+      <c r="F185" t="inlineStr"/>
+      <c r="G185" t="inlineStr"/>
+      <c r="H185" t="inlineStr"/>
+      <c r="I185" t="inlineStr"/>
+      <c r="J185" t="inlineStr"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>um parto de viagem</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>7,5</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr"/>
+      <c r="F186" t="inlineStr"/>
+      <c r="G186" t="inlineStr"/>
+      <c r="H186" t="inlineStr"/>
+      <c r="I186" t="inlineStr"/>
+      <c r="J186" t="inlineStr"/>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>o jogo da imitação</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr"/>
+      <c r="F187" t="inlineStr"/>
+      <c r="G187" t="inlineStr"/>
+      <c r="H187" t="inlineStr"/>
+      <c r="I187" t="inlineStr"/>
+      <c r="J187" t="inlineStr"/>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>bem vindo à prisão</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>8,2</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr"/>
+      <c r="F188" t="inlineStr"/>
+      <c r="G188" t="inlineStr"/>
+      <c r="H188" t="inlineStr"/>
+      <c r="I188" t="inlineStr"/>
+      <c r="J188" t="inlineStr"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>garota infernal</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>7,5</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr"/>
+      <c r="F189" t="inlineStr"/>
+      <c r="G189" t="inlineStr"/>
+      <c r="H189" t="inlineStr"/>
+      <c r="I189" t="inlineStr"/>
+      <c r="J189" t="inlineStr"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>defendor</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr"/>
+      <c r="F190" t="inlineStr"/>
+      <c r="G190" t="inlineStr"/>
+      <c r="H190" t="inlineStr"/>
+      <c r="I190" t="inlineStr"/>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>dropado</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>agente 86</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>8'</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr"/>
+      <c r="F191" t="inlineStr"/>
+      <c r="G191" t="inlineStr"/>
+      <c r="H191" t="inlineStr"/>
+      <c r="I191" t="inlineStr"/>
+      <c r="J191" t="inlineStr"/>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Tiras, só que não</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr"/>
+      <c r="F192" t="inlineStr"/>
+      <c r="G192" t="inlineStr"/>
+      <c r="H192" t="inlineStr"/>
+      <c r="I192" t="inlineStr"/>
+      <c r="J192" t="inlineStr"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>homem aranha no aranhaverso</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>9,8</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr"/>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr"/>
+      <c r="H193" t="inlineStr"/>
+      <c r="I193" t="inlineStr"/>
+      <c r="J193" t="inlineStr"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>olhos famintos</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr"/>
+      <c r="F194" t="inlineStr"/>
+      <c r="G194" t="inlineStr"/>
+      <c r="H194" t="inlineStr"/>
+      <c r="I194" t="inlineStr"/>
+      <c r="J194" t="inlineStr"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>O operário</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>8,5</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr"/>
+      <c r="F195" t="inlineStr"/>
+      <c r="G195" t="inlineStr"/>
+      <c r="H195" t="inlineStr"/>
+      <c r="I195" t="inlineStr"/>
+      <c r="J195" t="inlineStr"/>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Halloween</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr"/>
+      <c r="F196" t="inlineStr"/>
+      <c r="G196" t="inlineStr"/>
+      <c r="H196" t="inlineStr"/>
+      <c r="I196" t="inlineStr"/>
+      <c r="J196" t="inlineStr"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Homem aranha sem volta pra casa</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr"/>
+      <c r="F197" t="inlineStr"/>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr"/>
+      <c r="I197" t="inlineStr"/>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>cinema</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>